<commit_message>
Feature - Calculate grid fees based on whether it is a local or non-local transaction
</commit_message>
<xml_diff>
--- a/hamlet/tables.xlsx
+++ b/hamlet/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge23nur\Documents\Python Scripts\HAMLET\hamlet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge23nur\Documents\Python Scripts\HAMLET-gitlab\hamlet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350FCF08-5E86-486B-AE3B-1990C9DC4B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C41D24-8992-4881-9532-79F71F3019C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" autoFilterDateGrouping="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="303">
   <si>
     <t>column</t>
   </si>
@@ -941,6 +941,12 @@
   </si>
   <si>
     <t>unit depends on plant</t>
+  </si>
+  <si>
+    <t>id_trade</t>
+  </si>
+  <si>
+    <t>unique ID of trade</t>
   </si>
 </sst>
 </file>
@@ -1085,9 +1091,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1125,7 +1131,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1231,7 +1237,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1373,7 +1379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1385,9 +1391,9 @@
   <sheetViews>
     <sheetView showOutlineSymbols="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -1403,51 +1409,51 @@
   <sheetViews>
     <sheetView showOutlineSymbols="0" topLeftCell="A145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="45.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
@@ -1455,8 +1461,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1507,18 +1513,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
@@ -1526,8 +1532,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1623,18 +1629,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>60</v>
       </c>
@@ -1642,8 +1648,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1722,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1763,18 +1769,18 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -1782,8 +1788,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1888,31 +1894,31 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +1953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -2025,19 +2031,19 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="55" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>28</v>
       </c>
@@ -2142,24 +2148,24 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2179,7 +2185,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -2219,24 +2225,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -2270,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -2287,24 +2293,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="82" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>28</v>
       </c>
@@ -2355,18 +2361,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:27" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>60</v>
       </c>
@@ -2374,8 +2380,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -2458,12 +2464,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>28</v>
       </c>
@@ -2546,19 +2552,19 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="97" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B98" s="17" t="s">
         <v>94</v>
       </c>
@@ -2567,33 +2573,33 @@
       <c r="E98" s="17"/>
       <c r="F98" s="17"/>
     </row>
-    <row r="99" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
       <c r="E99" s="17"/>
       <c r="F99" s="17"/>
     </row>
-    <row r="100" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
       <c r="E100" s="17"/>
       <c r="F100" s="17"/>
     </row>
-    <row r="101" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="106" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -2635,19 +2641,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="111" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B113" s="17" t="s">
         <v>53</v>
       </c>
@@ -2656,33 +2662,33 @@
       <c r="E113" s="17"/>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
       <c r="D114" s="17"/>
       <c r="E114" s="17"/>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
       <c r="D115" s="17"/>
       <c r="E115" s="17"/>
       <c r="F115" s="17"/>
     </row>
-    <row r="116" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="121" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>28</v>
       </c>
@@ -2724,18 +2730,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="1:6" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="126" spans="1:6" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>185</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>60</v>
       </c>
@@ -2751,8 +2757,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="131" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>28</v>
       </c>
@@ -2857,13 +2863,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:29" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>186</v>
       </c>
@@ -2871,12 +2877,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="V138" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>42</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>28</v>
       </c>
@@ -3143,18 +3149,18 @@
         <v>184</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:29" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="144" spans="1:29" s="4" customFormat="1" ht="15.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="144" spans="1:29" s="4" customFormat="1" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A144" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>226</v>
       </c>
@@ -3162,7 +3168,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="147" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>60</v>
       </c>
@@ -3170,8 +3176,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="148" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="149" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="150" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>28</v>
       </c>
@@ -3231,13 +3237,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="152" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>230</v>
       </c>
@@ -3245,7 +3251,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="156" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
         <v>60</v>
       </c>
@@ -3253,8 +3259,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="157" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="158" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="159" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>28</v>
       </c>
@@ -3284,13 +3290,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="161" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>231</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="165" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
         <v>60</v>
       </c>
@@ -3306,8 +3312,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="166" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="167" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -3318,7 +3324,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="168" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -3329,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>28</v>
       </c>
@@ -3337,13 +3343,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="170" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>233</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="174" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
         <v>60</v>
       </c>
@@ -3359,8 +3365,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="175" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="176" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -3371,7 +3377,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="177" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>42</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>28</v>
       </c>
@@ -3390,13 +3396,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="179" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>237</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="183" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
         <v>60</v>
       </c>
@@ -3412,8 +3418,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="184" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="185" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="186" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>42</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>28</v>
       </c>
@@ -3491,13 +3497,13 @@
         <v>241</v>
       </c>
     </row>
-    <row r="188" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>242</v>
       </c>
@@ -3505,7 +3511,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="192" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="s">
         <v>60</v>
       </c>
@@ -3513,8 +3519,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="193" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="194" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>0</v>
       </c>
@@ -3525,7 +3531,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="195" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>42</v>
       </c>
@@ -3536,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>28</v>
       </c>
@@ -3544,12 +3550,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="197" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="1:3" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B98:F100"/>
@@ -3563,18 +3569,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845B957E-FD5F-4D07-9D0A-3E5DB720F61E}">
-  <dimension ref="A1:AK214"/>
+  <dimension ref="A1:AL214"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="AE33" sqref="AE33"/>
+      <selection activeCell="AL29" sqref="AL29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.7265625" defaultRowHeight="14.5" outlineLevelRow="4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="3"/>
+    <col min="1" max="1" width="25.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>282</v>
       </c>
@@ -3582,7 +3588,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>284</v>
       </c>
@@ -3599,7 +3605,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>97</v>
       </c>
@@ -3616,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>288</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>136</v>
       </c>
@@ -3650,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>140</v>
       </c>
@@ -3667,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>285</v>
       </c>
@@ -3684,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>138</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>171</v>
       </c>
@@ -3718,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>173</v>
       </c>
@@ -3735,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>174</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>203</v>
       </c>
@@ -3769,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>204</v>
       </c>
@@ -3786,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>205</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>182</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>206</v>
       </c>
@@ -3837,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>258</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>259</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>260</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>261</v>
       </c>
@@ -3905,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>266</v>
       </c>
@@ -3922,15 +3928,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="8"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:37" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>112</v>
       </c>
@@ -4042,8 +4048,11 @@
       <c r="AK26" s="9" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="27" spans="1:37" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="AL26" s="9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>28</v>
       </c>
@@ -4155,8 +4164,11 @@
       <c r="AK27" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="28" spans="1:37" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="AL27" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>111</v>
       </c>
@@ -4269,7 +4281,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:37" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" s="9" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>1</v>
       </c>
@@ -4381,16 +4393,19 @@
       <c r="AK29" s="9" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="30" spans="1:37" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL29" s="9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>169</v>
       </c>
@@ -4443,7 +4458,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>123</v>
       </c>
@@ -4484,7 +4499,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>124</v>
       </c>
@@ -4525,7 +4540,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>129</v>
       </c>
@@ -4533,7 +4548,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>130</v>
       </c>
@@ -4541,19 +4556,19 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="8"/>
       <c r="B38" s="13"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B42" s="5"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -4575,7 +4590,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="44" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="str">
         <f>A4</f>
         <v>balancing_energy</v>
@@ -4597,10 +4612,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -4649,7 +4664,7 @@
         <v>price_out</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -4699,7 +4714,7 @@
         <v>int64</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -4749,7 +4764,7 @@
         <v>€e7</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="9" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="9" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -4799,10 +4814,10 @@
         <v>total price for outflowing energy</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="8"/>
     </row>
-    <row r="52" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -4824,7 +4839,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="str">
         <f>A5</f>
         <v>timetable</v>
@@ -4846,14 +4861,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="D55" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -4902,7 +4917,7 @@
         <v>coupling</v>
       </c>
     </row>
-    <row r="57" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -4955,7 +4970,7 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
     </row>
-    <row r="58" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -5008,7 +5023,7 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
     </row>
-    <row r="59" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -5058,13 +5073,13 @@
         <v>coupling method (above, below)</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -5086,7 +5101,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="63" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="str">
         <f>A6</f>
         <v>market_transactions</v>
@@ -5108,10 +5123,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A64"/>
     </row>
-    <row r="65" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -5176,7 +5191,7 @@
         <v>share_quality_XXX</v>
       </c>
     </row>
-    <row r="66" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -5242,7 +5257,7 @@
         <v>int8</v>
       </c>
     </row>
-    <row r="67" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -5308,7 +5323,7 @@
         <v>0-100</v>
       </c>
     </row>
-    <row r="68" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -5374,10 +5389,10 @@
         <v>quality share of energy (one column per type)</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="8"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -5399,7 +5414,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="72" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="str">
         <f>A7</f>
         <v>meter_readings_cum</v>
@@ -5421,10 +5436,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A73"/>
     </row>
-    <row r="74" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -5461,7 +5476,7 @@
         <v>energy_out</v>
       </c>
     </row>
-    <row r="75" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -5499,7 +5514,7 @@
         <v>uint64</v>
       </c>
     </row>
-    <row r="76" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -5537,7 +5552,7 @@
         <v>Wh</v>
       </c>
     </row>
-    <row r="77" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -5575,10 +5590,10 @@
         <v>energy going out of the meter</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="8"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -5600,7 +5615,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="81" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="str">
         <f>A8</f>
         <v>meter_readings_delta</v>
@@ -5622,10 +5637,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -5662,7 +5677,7 @@
         <v>energy_out</v>
       </c>
     </row>
-    <row r="84" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -5700,7 +5715,7 @@
         <v>uint64</v>
       </c>
     </row>
-    <row r="85" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -5738,7 +5753,7 @@
         <v>Wh</v>
       </c>
     </row>
-    <row r="86" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -5776,10 +5791,10 @@
         <v>energy going out of the meter</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="8"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -5801,7 +5816,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="90" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A90" s="16" t="s">
         <v>138</v>
       </c>
@@ -5822,10 +5837,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A91"/>
     </row>
-    <row r="92" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -5878,7 +5893,7 @@
         <v>price_out</v>
       </c>
     </row>
-    <row r="93" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -5932,7 +5947,7 @@
         <v>int64</v>
       </c>
     </row>
-    <row r="94" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -5986,7 +6001,7 @@
         <v>€e7</v>
       </c>
     </row>
-    <row r="95" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -6040,10 +6055,10 @@
         <v>total price for outflowing energy</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="8"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -6065,7 +6080,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="99" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A99" s="16" t="s">
         <v>171</v>
       </c>
@@ -6086,10 +6101,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A100"/>
     </row>
-    <row r="101" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -6146,7 +6161,7 @@
         <v>share_quality_XXX</v>
       </c>
     </row>
-    <row r="102" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -6204,7 +6219,7 @@
         <v>int8</v>
       </c>
     </row>
-    <row r="103" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -6262,7 +6277,7 @@
         <v>0-100</v>
       </c>
     </row>
-    <row r="104" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -6320,10 +6335,10 @@
         <v>quality share of energy (one column per type)</v>
       </c>
     </row>
-    <row r="105" spans="1:14" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="8"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -6345,7 +6360,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="108" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A108" s="16" t="s">
         <v>173</v>
       </c>
@@ -6366,10 +6381,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A109"/>
     </row>
-    <row r="110" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -6422,7 +6437,7 @@
         <v>type_plants</v>
       </c>
     </row>
-    <row r="111" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -6476,7 +6491,7 @@
         <v>categorical</v>
       </c>
     </row>
-    <row r="112" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -6530,7 +6545,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="113" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -6584,10 +6599,10 @@
         <v>types of plants (per agent)</v>
       </c>
     </row>
-    <row r="114" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="8"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -6609,7 +6624,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="117" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A117" s="16" t="s">
         <v>174</v>
       </c>
@@ -6630,10 +6645,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A118"/>
     </row>
-    <row r="119" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -6666,7 +6681,7 @@
         <v>quality</v>
       </c>
     </row>
-    <row r="120" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -6706,7 +6721,7 @@
       <c r="M120" s="3"/>
       <c r="N120" s="3"/>
     </row>
-    <row r="121" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -6746,7 +6761,7 @@
       <c r="M121" s="3"/>
       <c r="N121" s="3"/>
     </row>
-    <row r="122" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -6780,10 +6795,10 @@
         <v>quality of energy</v>
       </c>
     </row>
-    <row r="123" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="8"/>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -6805,7 +6820,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="126" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>203</v>
       </c>
@@ -6826,10 +6841,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A127"/>
     </row>
-    <row r="128" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -6876,7 +6891,7 @@
       <c r="N128" s="9"/>
       <c r="O128" s="9"/>
     </row>
-    <row r="129" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -6924,7 +6939,7 @@
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
     </row>
-    <row r="130" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -6972,7 +6987,7 @@
       <c r="N130" s="3"/>
       <c r="O130" s="3"/>
     </row>
-    <row r="131" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -7018,10 +7033,10 @@
         <v>total price for incoming energy</v>
       </c>
     </row>
-    <row r="132" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A132" s="8"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -7043,7 +7058,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="135" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A135" s="16" t="s">
         <v>204</v>
       </c>
@@ -7064,10 +7079,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A136"/>
     </row>
-    <row r="137" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -7112,7 +7127,7 @@
         <v>price_in</v>
       </c>
     </row>
-    <row r="138" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A138" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -7161,7 +7176,7 @@
       <c r="N138" s="3"/>
       <c r="O138" s="3"/>
     </row>
-    <row r="139" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -7210,7 +7225,7 @@
       <c r="N139" s="3"/>
       <c r="O139" s="3"/>
     </row>
-    <row r="140" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -7256,10 +7271,10 @@
         <v>total price for incoming energy</v>
       </c>
     </row>
-    <row r="141" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" s="8"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A143" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -7281,7 +7296,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="144" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A144" s="16" t="s">
         <v>205</v>
       </c>
@@ -7302,10 +7317,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A145"/>
     </row>
-    <row r="146" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -7354,7 +7369,7 @@
         <v>quality</v>
       </c>
     </row>
-    <row r="147" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A147" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -7406,7 +7421,7 @@
       <c r="N147" s="3"/>
       <c r="O147" s="3"/>
     </row>
-    <row r="148" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A148" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -7458,7 +7473,7 @@
       <c r="N148" s="3"/>
       <c r="O148" s="3"/>
     </row>
-    <row r="149" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A149" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -7508,10 +7523,10 @@
         <v>quality of energy</v>
       </c>
     </row>
-    <row r="150" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A150" s="8"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A152" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -7533,7 +7548,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="153" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="s">
         <v>182</v>
       </c>
@@ -7554,10 +7569,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A154"/>
     </row>
-    <row r="155" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -7606,7 +7621,7 @@
         <v>quality</v>
       </c>
     </row>
-    <row r="156" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A156" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -7659,7 +7674,7 @@
       <c r="N156" s="3"/>
       <c r="O156" s="3"/>
     </row>
-    <row r="157" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A157" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -7712,7 +7727,7 @@
       <c r="N157" s="3"/>
       <c r="O157" s="3"/>
     </row>
-    <row r="158" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A158" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -7762,10 +7777,10 @@
         <v>quality of energy</v>
       </c>
     </row>
-    <row r="159" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="8"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A161" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -7787,7 +7802,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="162" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A162" s="16" t="s">
         <v>206</v>
       </c>
@@ -7808,10 +7823,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A163"/>
     </row>
-    <row r="164" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -7864,7 +7879,7 @@
         <v>quality</v>
       </c>
     </row>
-    <row r="165" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A165" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -7920,7 +7935,7 @@
       <c r="N165" s="3"/>
       <c r="O165" s="3"/>
     </row>
-    <row r="166" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A166" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -7976,7 +7991,7 @@
       <c r="N166" s="3"/>
       <c r="O166" s="3"/>
     </row>
-    <row r="167" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A167" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8030,10 +8045,10 @@
         <v>quality of energy</v>
       </c>
     </row>
-    <row r="168" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" s="8"/>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A170" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -8055,7 +8070,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="171" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A171" s="16" t="s">
         <v>258</v>
       </c>
@@ -8076,13 +8091,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A172"/>
       <c r="B172" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="173" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -8097,7 +8112,7 @@
       <c r="L173" s="9"/>
       <c r="M173" s="9"/>
     </row>
-    <row r="174" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A174" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -8120,7 +8135,7 @@
       <c r="N174" s="3"/>
       <c r="O174" s="3"/>
     </row>
-    <row r="175" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A175" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -8143,7 +8158,7 @@
       <c r="N175" s="3"/>
       <c r="O175" s="3"/>
     </row>
-    <row r="176" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A176" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8153,10 +8168,10 @@
         <v>used energy over all timesteps</v>
       </c>
     </row>
-    <row r="177" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" s="8"/>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A179" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -8178,7 +8193,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="180" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A180" s="16" t="s">
         <v>259</v>
       </c>
@@ -8199,13 +8214,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A181"/>
       <c r="B181" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="182" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -8220,7 +8235,7 @@
       <c r="L182" s="9"/>
       <c r="M182" s="9"/>
     </row>
-    <row r="183" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A183" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -8243,7 +8258,7 @@
       <c r="N183" s="3"/>
       <c r="O183" s="3"/>
     </row>
-    <row r="184" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A184" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -8266,7 +8281,7 @@
       <c r="N184" s="3"/>
       <c r="O184" s="3"/>
     </row>
-    <row r="185" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A185" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8276,10 +8291,10 @@
         <v>state-of-charge</v>
       </c>
     </row>
-    <row r="186" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A186" s="8"/>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A188" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -8301,7 +8316,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="189" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A189" s="16" t="s">
         <v>260</v>
       </c>
@@ -8322,13 +8337,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A190"/>
       <c r="C190" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="191" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -8347,7 +8362,7 @@
       <c r="L191" s="9"/>
       <c r="M191" s="9"/>
     </row>
-    <row r="192" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A192" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -8373,7 +8388,7 @@
       <c r="N192" s="3"/>
       <c r="O192" s="3"/>
     </row>
-    <row r="193" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A193" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -8399,7 +8414,7 @@
       <c r="N193" s="3"/>
       <c r="O193" s="3"/>
     </row>
-    <row r="194" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A194" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8413,10 +8428,10 @@
         <v>value of plant timeseries</v>
       </c>
     </row>
-    <row r="195" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A195" s="8"/>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A197" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -8438,7 +8453,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="198" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A198" s="16" t="s">
         <v>261</v>
       </c>
@@ -8459,13 +8474,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A199"/>
       <c r="D199" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="200" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -8482,7 +8497,7 @@
         <v>power</v>
       </c>
     </row>
-    <row r="201" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A201" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -8511,7 +8526,7 @@
       <c r="N201" s="3"/>
       <c r="O201" s="3"/>
     </row>
-    <row r="202" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A202" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -8540,7 +8555,7 @@
       <c r="N202" s="3"/>
       <c r="O202" s="3"/>
     </row>
-    <row r="203" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A203" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8558,10 +8573,10 @@
         <v>undirectional power</v>
       </c>
     </row>
-    <row r="204" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A204" s="8"/>
     </row>
-    <row r="206" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A206" s="15" t="str">
         <f>$A$3</f>
         <v>Table</v>
@@ -8583,7 +8598,7 @@
         <v>Saved</v>
       </c>
     </row>
-    <row r="207" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="16" t="str">
         <f>A22</f>
         <v>forecasts</v>
@@ -8605,14 +8620,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35"/>
+    <row r="209" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A209"/>
       <c r="D209" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="210" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -8635,7 +8650,7 @@
       <c r="L210" s="9"/>
       <c r="M210" s="9"/>
     </row>
-    <row r="211" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A211" s="9" t="str">
         <f>$A$27</f>
         <v>dtype</v>
@@ -8664,7 +8679,7 @@
       <c r="N211" s="3"/>
       <c r="O211" s="3"/>
     </row>
-    <row r="212" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A212" s="9" t="str">
         <f>$A$28</f>
         <v>unit</v>
@@ -8693,7 +8708,7 @@
       <c r="N212" s="3"/>
       <c r="O212" s="3"/>
     </row>
-    <row r="213" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A213" s="9" t="str">
         <f>$A$29</f>
         <v>description</v>
@@ -8711,7 +8726,7 @@
         <v>value of plant timeseries</v>
       </c>
     </row>
-    <row r="214" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A214" s="8"/>
     </row>
   </sheetData>

</xml_diff>